<commit_message>
a few new changes on a mac computer
</commit_message>
<xml_diff>
--- a/code/Appendix3_maxentParameters_v2.xlsx
+++ b/code/Appendix3_maxentParameters_v2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="226">
   <si>
     <t>ID</t>
   </si>
@@ -413,9 +413,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>Description of parameter</t>
   </si>
   <si>
     <t>Create graphs showing how predicted relative probability of occurrence depends on the value of each environmental variable.</t>
@@ -689,26 +686,32 @@
 Maximum training sensitivity plus specificity.</t>
   </si>
   <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>An overview of Maxent parameters and their implementations in R.</t>
+  </si>
+  <si>
+    <t>Description of parameter*</t>
+  </si>
+  <si>
     <t>Parameters in Maxent
-(or flag)</t>
+(or flag*)</t>
   </si>
   <si>
     <t>Abbreviation
-of parameters</t>
+of parameters*</t>
   </si>
   <si>
     <t>Type of 
-parameter</t>
+parameter*</t>
   </si>
   <si>
     <t>Default value 
-in Maxent</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>An overview of Maxent parameters and their implementations in R.</t>
+in Maxent*</t>
+  </si>
+  <si>
+    <t>*Note: information is directly from Maxent help document.</t>
   </si>
 </sst>
 </file>
@@ -1597,17 +1600,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.06640625" style="6"/>
     <col min="2" max="2" width="25.1328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.9296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.06640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.06640625" style="5" bestFit="1" customWidth="1"/>
@@ -1617,7 +1620,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.45">
@@ -1625,28 +1628,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>132</v>
-      </c>
       <c r="G2" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -1666,16 +1669,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -1686,7 +1689,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>3</v>
@@ -1695,16 +1698,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -1724,16 +1727,16 @@
         <v>0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -1744,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>8</v>
@@ -1753,16 +1756,16 @@
         <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H6" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -1773,7 +1776,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>8</v>
@@ -1782,16 +1785,16 @@
         <v>11</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -1808,19 +1811,19 @@
         <v>14</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="93.6" x14ac:dyDescent="0.45">
@@ -1837,19 +1840,19 @@
         <v>18</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -1866,19 +1869,19 @@
         <v>22</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -1895,19 +1898,19 @@
         <v>18</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -1918,7 +1921,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>3</v>
@@ -1930,13 +1933,13 @@
         <v>28</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H12" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -1947,7 +1950,7 @@
         <v>29</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>3</v>
@@ -1959,13 +1962,13 @@
         <v>30</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -1976,7 +1979,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>3</v>
@@ -1988,13 +1991,13 @@
         <v>32</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2005,7 +2008,7 @@
         <v>33</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>3</v>
@@ -2014,16 +2017,16 @@
         <v>1</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -2046,13 +2049,13 @@
         <v>36</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2075,13 +2078,13 @@
         <v>39</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -2092,7 +2095,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>3</v>
@@ -2104,13 +2107,13 @@
         <v>41</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -2121,7 +2124,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>3</v>
@@ -2133,13 +2136,13 @@
         <v>43</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="93.6" x14ac:dyDescent="0.45">
@@ -2150,7 +2153,7 @@
         <v>44</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>3</v>
@@ -2162,13 +2165,13 @@
         <v>45</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2191,13 +2194,13 @@
         <v>49</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2217,16 +2220,16 @@
         <v>1</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -2246,16 +2249,16 @@
         <v>10000</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="93.6" x14ac:dyDescent="0.45">
@@ -2266,25 +2269,25 @@
         <v>55</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -2301,19 +2304,19 @@
         <v>22</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>58</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2324,7 +2327,7 @@
         <v>59</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>48</v>
@@ -2333,16 +2336,16 @@
         <v>1</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H26" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="I26" s="7" t="s">
         <v>197</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="140.4" x14ac:dyDescent="0.45">
@@ -2353,7 +2356,7 @@
         <v>60</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>8</v>
@@ -2365,13 +2368,13 @@
         <v>62</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H27" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="I27" s="7" t="s">
         <v>199</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
@@ -2382,7 +2385,7 @@
         <v>63</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>3</v>
@@ -2391,16 +2394,16 @@
         <v>0</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
@@ -2411,7 +2414,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>3</v>
@@ -2420,16 +2423,16 @@
         <v>0</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2440,7 +2443,7 @@
         <v>65</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>3</v>
@@ -2449,16 +2452,16 @@
         <v>0</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -2478,13 +2481,13 @@
         <v>1</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I31" s="7" t="s">
         <v>129</v>
@@ -2507,13 +2510,13 @@
         <v>1</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I32" s="7" t="s">
         <v>130</v>
@@ -2536,13 +2539,13 @@
         <v>1</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>2</v>
@@ -2556,7 +2559,7 @@
         <v>72</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>3</v>
@@ -2565,13 +2568,13 @@
         <v>1</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I34" s="7" t="s">
         <v>57</v>
@@ -2594,13 +2597,13 @@
         <v>1</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I35" s="7" t="s">
         <v>131</v>
@@ -2623,16 +2626,16 @@
         <v>1</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -2643,7 +2646,7 @@
         <v>77</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>3</v>
@@ -2652,16 +2655,16 @@
         <v>0</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
@@ -2681,16 +2684,16 @@
         <v>0</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2701,7 +2704,7 @@
         <v>80</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>3</v>
@@ -2710,16 +2713,16 @@
         <v>0</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H39" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="I39" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2730,7 +2733,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>3</v>
@@ -2739,16 +2742,16 @@
         <v>0</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2759,7 +2762,7 @@
         <v>82</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>3</v>
@@ -2768,16 +2771,16 @@
         <v>1</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
@@ -2797,16 +2800,16 @@
         <v>1</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2826,16 +2829,16 @@
         <v>1</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -2846,7 +2849,7 @@
         <v>87</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>3</v>
@@ -2855,16 +2858,16 @@
         <v>1</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H44" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="I44" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="I44" s="7" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -2887,13 +2890,13 @@
         <v>90</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
@@ -2904,7 +2907,7 @@
         <v>91</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>3</v>
@@ -2913,16 +2916,16 @@
         <v>1</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
@@ -2933,7 +2936,7 @@
         <v>92</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>3</v>
@@ -2942,16 +2945,16 @@
         <v>0</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -2971,16 +2974,16 @@
         <v>500</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3000,16 +3003,16 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -3020,7 +3023,7 @@
         <v>97</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>48</v>
@@ -3032,13 +3035,13 @@
         <v>98</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -3049,7 +3052,7 @@
         <v>99</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>48</v>
@@ -3061,13 +3064,13 @@
         <v>100</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3078,7 +3081,7 @@
         <v>101</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>48</v>
@@ -3087,16 +3090,16 @@
         <v>80</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
@@ -3107,7 +3110,7 @@
         <v>102</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>48</v>
@@ -3116,16 +3119,16 @@
         <v>10</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
@@ -3136,7 +3139,7 @@
         <v>103</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>48</v>
@@ -3145,16 +3148,16 @@
         <v>15</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3165,7 +3168,7 @@
         <v>104</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>52</v>
@@ -3174,16 +3177,16 @@
         <v>-1</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3194,7 +3197,7 @@
         <v>105</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>52</v>
@@ -3203,16 +3206,16 @@
         <v>-1</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3223,7 +3226,7 @@
         <v>106</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>52</v>
@@ -3232,16 +3235,16 @@
         <v>-1</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3252,7 +3255,7 @@
         <v>107</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>52</v>
@@ -3261,16 +3264,16 @@
         <v>-1</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3281,7 +3284,7 @@
         <v>108</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>8</v>
@@ -3290,16 +3293,16 @@
         <v>109</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
@@ -3310,7 +3313,7 @@
         <v>110</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>3</v>
@@ -3319,16 +3322,16 @@
         <v>1</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="70.2" x14ac:dyDescent="0.45">
@@ -3339,7 +3342,7 @@
         <v>111</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>52</v>
@@ -3351,13 +3354,13 @@
         <v>112</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="187.2" x14ac:dyDescent="0.45">
@@ -3368,25 +3371,25 @@
         <v>113</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>114</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3403,19 +3406,19 @@
         <v>8</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3432,19 +3435,19 @@
         <v>8</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3461,19 +3464,19 @@
         <v>8</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
@@ -3493,16 +3496,16 @@
         <v>0</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3513,7 +3516,7 @@
         <v>123</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>3</v>
@@ -3525,13 +3528,13 @@
         <v>124</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
@@ -3542,7 +3545,7 @@
         <v>125</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>3</v>
@@ -3554,13 +3557,13 @@
         <v>126</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
@@ -3580,16 +3583,21 @@
         <v>-9999</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A70" s="4" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>